<commit_message>
cap 1, refs, motiv
</commit_message>
<xml_diff>
--- a/assets/functions_list.xlsx
+++ b/assets/functions_list.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c7dd956b4cb9528e/Alpha Drive/Trabalho/Programming/Curso_R/CursoR_LectureNotes/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="8_{81E7AC61-A3EA-49FC-B5AC-4DE96DB90C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D686967-8B3D-4C83-A59E-E65338941D56}"/>
+  <xr:revisionPtr revIDLastSave="284" documentId="8_{81E7AC61-A3EA-49FC-B5AC-4DE96DB90C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44E6B6CF-2407-47BC-A488-3D51A6BA95DF}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{06F320C8-D750-4D9F-AB12-575DC64BD434}"/>
+    <workbookView xWindow="-21720" yWindow="915" windowWidth="21840" windowHeight="13140" xr2:uid="{06F320C8-D750-4D9F-AB12-575DC64BD434}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="lista" sheetId="3" r:id="rId1"/>
+    <sheet name="operadores" sheetId="1" r:id="rId2"/>
+    <sheet name="precedência" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,286 +38,477 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="89">
-  <si>
-    <t>[+](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Arithmetic.html)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="151">
   <si>
     <t>soma</t>
   </si>
   <si>
-    <t>[-](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Arithmetic.html)</t>
-  </si>
-  <si>
     <t>subtração</t>
   </si>
   <si>
-    <t>[*](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Arithmetic.html)</t>
-  </si>
-  <si>
     <t>multiplicação</t>
   </si>
   <si>
-    <t>[/](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Arithmetic.html)</t>
-  </si>
-  <si>
     <t>divisão</t>
   </si>
   <si>
-    <t>[\^](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Arithmetic.html)</t>
-  </si>
-  <si>
     <t>exponenciação</t>
   </si>
   <si>
-    <t>[%%](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Arithmetic.html)</t>
-  </si>
-  <si>
     <t>divisão inteira</t>
   </si>
   <si>
-    <t>[%/%](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Arithmetic.html)</t>
-  </si>
-  <si>
     <t>resto da divisão</t>
   </si>
   <si>
-    <t>[(](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Paren.html)</t>
-  </si>
-  <si>
-    <t>parênteses</t>
-  </si>
-  <si>
-    <t>num `+` num</t>
-  </si>
-  <si>
-    <t>num `-` num</t>
-  </si>
-  <si>
-    <t>num `*` num</t>
-  </si>
-  <si>
-    <t>num `/` num</t>
-  </si>
-  <si>
-    <t>num `^` num</t>
-  </si>
-  <si>
-    <t>num `%%` num</t>
-  </si>
-  <si>
-    <t>num `%/%` num</t>
-  </si>
-  <si>
-    <t>`(` expr `)`</t>
-  </si>
-  <si>
-    <t>aritmetrics</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Function</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Usage</t>
-  </si>
-  <si>
-    <t>Chapter</t>
-  </si>
-  <si>
-    <t>[==](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Comparison.html)</t>
-  </si>
-  <si>
     <t>igual</t>
   </si>
   <si>
-    <t>x == y</t>
-  </si>
-  <si>
-    <t>[!=](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Comparison.html)</t>
-  </si>
-  <si>
     <t>diferente</t>
   </si>
   <si>
-    <t>x !=  y</t>
-  </si>
-  <si>
-    <t>[&lt;](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Comparison.html)</t>
-  </si>
-  <si>
     <t>menor que</t>
   </si>
   <si>
-    <t>[&gt;](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Comparison.html)</t>
-  </si>
-  <si>
     <t>maior que</t>
   </si>
   <si>
-    <t>[&gt;=](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Comparison.html)</t>
-  </si>
-  <si>
     <t>maior igual</t>
   </si>
   <si>
-    <t>x &gt;=  y</t>
-  </si>
-  <si>
-    <t>[&lt;=](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Comparison.html)</t>
-  </si>
-  <si>
     <t>menor igual</t>
   </si>
   <si>
-    <t>x &lt;=  y</t>
-  </si>
-  <si>
-    <t>[!](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Logic.html)</t>
-  </si>
-  <si>
-    <t>negação</t>
-  </si>
-  <si>
-    <t>! logi</t>
-  </si>
-  <si>
-    <t>[&amp;](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Logic.html)</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>logi &amp; logi</t>
-  </si>
-  <si>
-    <t>[|](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Logic.html)</t>
-  </si>
-  <si>
-    <t>ou</t>
-  </si>
-  <si>
-    <t>logi | logi</t>
-  </si>
-  <si>
-    <t>[&amp;&amp;](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Logic.html)</t>
-  </si>
-  <si>
-    <t>e singular</t>
-  </si>
-  <si>
-    <t>logi &amp;&amp; logi</t>
-  </si>
-  <si>
-    <t>[||](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Logic.html)</t>
-  </si>
-  <si>
-    <t>ou singular</t>
-  </si>
-  <si>
-    <t>logi || logi</t>
-  </si>
-  <si>
-    <t>[%in%](https://stat.ethz.ch/R-manual/R-devel/library/base/html/match.html)</t>
-  </si>
-  <si>
     <t>pertence/está contido</t>
   </si>
   <si>
     <t>vector %in% vector</t>
   </si>
   <si>
-    <t>[~](https://stat.ethz.ch/R-manual/R-devel/library/base/html/tilde.html)</t>
-  </si>
-  <si>
     <t>operador til</t>
   </si>
   <si>
-    <t>[%*%](https://stat.ethz.ch/R-manual/R-devel/library/base/html/matmult.html)</t>
-  </si>
-  <si>
     <t>Matrix Multiplication</t>
   </si>
   <si>
     <t>matrix %*% matrix</t>
   </si>
   <si>
-    <t>[%o%](https://stat.ethz.ch/R-manual/R-devel/library/base/html/outer.html)</t>
-  </si>
-  <si>
     <t>Outer Product of Arrays</t>
   </si>
   <si>
     <t>matrix %o% matrix</t>
   </si>
   <si>
-    <t>[%x%](https://stat.ethz.ch/R-manual/R-devel/library/base/html/kronecker.html)</t>
-  </si>
-  <si>
     <t>Kronecker Products on Arrays</t>
   </si>
   <si>
     <t>matrix %x% matrix</t>
   </si>
   <si>
-    <t>[|&gt;](https://stat.ethz.ch/R-manual/R-devel/library/base/html/pipeOp.html)</t>
-  </si>
-  <si>
     <t>Forward Pipe Operator</t>
   </si>
   <si>
     <t>call |&gt; call</t>
   </si>
   <si>
-    <t>[:](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Colon.html)</t>
-  </si>
-  <si>
     <t>Colon Operator</t>
   </si>
   <si>
     <t>num:num</t>
   </si>
   <si>
-    <t>[::](https://stat.ethz.ch/R-manual/R-devel/library/base/html/ns-dblcolon.html)</t>
-  </si>
-  <si>
     <t>Double Colon and Triple Colon Operators</t>
   </si>
   <si>
     <t>pkg::fun</t>
   </si>
   <si>
-    <t>[:::](https://stat.ethz.ch/R-manual/R-devel/library/base/html/ns-dblcolon.html)</t>
-  </si>
-  <si>
     <t>pkg:::fun</t>
   </si>
   <si>
-    <t>logical</t>
-  </si>
-  <si>
-    <t>comparison</t>
-  </si>
-  <si>
     <t>matrix</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>~ (unary and binary)</t>
+  </si>
+  <si>
+    <t>::, :::</t>
+  </si>
+  <si>
+    <t>$, @</t>
+  </si>
+  <si>
+    <t>-, + (unary)</t>
+  </si>
+  <si>
+    <t>*, /</t>
+  </si>
+  <si>
+    <t>+, - (binary)</t>
+  </si>
+  <si>
+    <t>&gt;, &gt;=, &lt;, &lt;=, ==, !=</t>
+  </si>
+  <si>
+    <t>&amp;, &amp;&amp;</t>
+  </si>
+  <si>
+    <t>|, ||</t>
+  </si>
+  <si>
+    <t>-&gt;, -&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;- ,&lt;&lt;-</t>
+  </si>
+  <si>
+    <t>%%, %/%, %xyz%, |&gt;</t>
+  </si>
+  <si>
+    <t>extração de _components_/_slots_ (*)</t>
+  </si>
+  <si>
+    <t>acessar _namespaces_ (*)</t>
+  </si>
+  <si>
+    <t>mais e menos unários</t>
+  </si>
+  <si>
+    <t>sequências (*)</t>
+  </si>
+  <si>
+    <t>multiplicação, divisão</t>
+  </si>
+  <si>
+    <t>adição, subtração</t>
+  </si>
+  <si>
+    <t>comparações</t>
+  </si>
+  <si>
+    <t>"não" lógico</t>
+  </si>
+  <si>
+    <t>"e" lógico</t>
+  </si>
+  <si>
+    <t>"ou" lógico</t>
+  </si>
+  <si>
+    <t>fórmula (*)</t>
+  </si>
+  <si>
+    <t>definição pra esquerda</t>
+  </si>
+  <si>
+    <t>= (definidor)</t>
+  </si>
+  <si>
+    <t>direita pra esquerda</t>
+  </si>
+  <si>
+    <t>esquerda pra direita</t>
+  </si>
+  <si>
+    <t>"e" lógico singular</t>
+  </si>
+  <si>
+    <t>"ou" lógico singular</t>
+  </si>
+  <si>
+    <t>logi `&amp;&amp;` logi</t>
+  </si>
+  <si>
+    <t>logi `||` logi</t>
+  </si>
+  <si>
+    <t>Capítulo</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Uso</t>
+  </si>
+  <si>
+    <t>aritmétrica</t>
+  </si>
+  <si>
+    <t>comparação</t>
+  </si>
+  <si>
+    <t>lógica</t>
+  </si>
+  <si>
+    <t>Operador</t>
+  </si>
+  <si>
+    <t>Descição</t>
+  </si>
+  <si>
+    <t>Associatividade</t>
+  </si>
+  <si>
+    <t>operadores especiais (*)</t>
+  </si>
+  <si>
+    <t>"e" lógico (*)</t>
+  </si>
+  <si>
+    <t>"ou" lógico (*)</t>
+  </si>
+  <si>
+    <t>definição pra direita (*)</t>
+  </si>
+  <si>
+    <t>definição pra esquerda (*)</t>
+  </si>
+  <si>
+    <t>[, [[</t>
+  </si>
+  <si>
+    <t>indexação (*)</t>
+  </si>
+  <si>
+    <t>(), {}</t>
+  </si>
+  <si>
+    <t>agrupadores</t>
+  </si>
+  <si>
+    <t>Função</t>
+  </si>
+  <si>
+    <t>`num + num`</t>
+  </si>
+  <si>
+    <t>`num - num`</t>
+  </si>
+  <si>
+    <t>`num * num`</t>
+  </si>
+  <si>
+    <t>`num / num`</t>
+  </si>
+  <si>
+    <t>`num ^ num`</t>
+  </si>
+  <si>
+    <t>`num %% num`</t>
+  </si>
+  <si>
+    <t>`num %/% num`</t>
+  </si>
+  <si>
+    <t>`( expr )`</t>
+  </si>
+  <si>
+    <t>`x == y`</t>
+  </si>
+  <si>
+    <t>`x !=  y`</t>
+  </si>
+  <si>
+    <t>`num &lt; num`</t>
+  </si>
+  <si>
+    <t>`num &gt; num`</t>
+  </si>
+  <si>
+    <t>`num &gt;=  num`</t>
+  </si>
+  <si>
+    <t>`num &lt;=  num`</t>
+  </si>
+  <si>
+    <t>`! logi`</t>
+  </si>
+  <si>
+    <t>`logi &amp; logi`</t>
+  </si>
+  <si>
+    <t>`logi | logi`</t>
+  </si>
+  <si>
+    <t>agrupador chaves</t>
+  </si>
+  <si>
+    <t>agrupador parênteses</t>
+  </si>
+  <si>
+    <t>`{ expr }`</t>
+  </si>
+  <si>
+    <t>[`+`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Arithmetic.html)</t>
+  </si>
+  <si>
+    <t>[`-`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Arithmetic.html)</t>
+  </si>
+  <si>
+    <t>[`*`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Arithmetic.html)</t>
+  </si>
+  <si>
+    <t>[`/`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Arithmetic.html)</t>
+  </si>
+  <si>
+    <t>[`\^`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Arithmetic.html)</t>
+  </si>
+  <si>
+    <t>[`%%`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Arithmetic.html)</t>
+  </si>
+  <si>
+    <t>[`%/%`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Arithmetic.html)</t>
+  </si>
+  <si>
+    <t>[`==`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Comparison.html)</t>
+  </si>
+  <si>
+    <t>[`!=`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Comparison.html)</t>
+  </si>
+  <si>
+    <t>[`&lt;`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Comparison.html)</t>
+  </si>
+  <si>
+    <t>[`&gt;`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Comparison.html)</t>
+  </si>
+  <si>
+    <t>[`&gt;=`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Comparison.html)</t>
+  </si>
+  <si>
+    <t>[`&lt;=`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Comparison.html)</t>
+  </si>
+  <si>
+    <t>[`!`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Logic.html)</t>
+  </si>
+  <si>
+    <t>[`&amp;`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Logic.html)</t>
+  </si>
+  <si>
+    <t>[`|`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Logic.html)</t>
+  </si>
+  <si>
+    <t>[`{`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Paren.html)</t>
+  </si>
+  <si>
+    <t>[`(`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Paren.html)</t>
+  </si>
+  <si>
+    <t>[`&amp;&amp;`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Logic.html)</t>
+  </si>
+  <si>
+    <t>[`||`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Logic.html)</t>
+  </si>
+  <si>
+    <t>[`%in%`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/match.html)</t>
+  </si>
+  <si>
+    <t>[`~`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/tilde.html)</t>
+  </si>
+  <si>
+    <t>[`%*%`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/matmult.html)</t>
+  </si>
+  <si>
+    <t>[`%o%`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/outer.html)</t>
+  </si>
+  <si>
+    <t>[`%x%`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/kronecker.html)</t>
+  </si>
+  <si>
+    <t>[`|&gt;`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/pipeOp.html)</t>
+  </si>
+  <si>
+    <t>[`:`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/Colon.html)</t>
+  </si>
+  <si>
+    <t>[`::`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/ns-dblcolon.html)</t>
+  </si>
+  <si>
+    <t>[`:::`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/ns-dblcolon.html)</t>
+  </si>
+  <si>
+    <t>definidores</t>
+  </si>
+  <si>
+    <t>[`rm()`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/rm.html)</t>
+  </si>
+  <si>
+    <t>[`&lt;-`, `-&gt;`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/assignOps.html)</t>
+  </si>
+  <si>
+    <t>[`=`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/assignOps.html)</t>
+  </si>
+  <si>
+    <t>`x &lt;- expr`, `x -&gt; expr`</t>
+  </si>
+  <si>
+    <t>`x = expr`</t>
+  </si>
+  <si>
+    <t>limpa objetos do ambiente</t>
+  </si>
+  <si>
+    <t>`rm(x)`</t>
+  </si>
+  <si>
+    <t>[`make.names()`](https://stat.ethz.ch/R-manual/R-devel/library/base/html/make.names.html)</t>
+  </si>
+  <si>
+    <t>[`help()`](https://stat.ethz.ch/R-manual/R-devel/library/utils/html/help.html), [`?`](https://stat.ethz.ch/R-manual/R-devel/library/utils/html/Question.html)</t>
+  </si>
+  <si>
+    <t>procurar ajuda na documentação</t>
+  </si>
+  <si>
+    <t>`help(x)`, `?x`</t>
+  </si>
+  <si>
+    <t>[`vignette()`](https://stat.ethz.ch/R-manual/R-devel/library/utils/html/vignette.html)</t>
+  </si>
+  <si>
+    <t>procurar vignettes</t>
+  </si>
+  <si>
+    <t>`vignette(x)`</t>
+  </si>
+  <si>
+    <t>ajuda</t>
+  </si>
+  <si>
+    <t>nomes</t>
+  </si>
+  <si>
+    <t>outros</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -338,8 +531,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,33 +875,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E450260-C86C-4E3F-B105-E3CAA65587BC}">
-  <dimension ref="A1:E29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C0DCBB-DBA4-4D59-AA5F-8E3DDFA0C851}">
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>83</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -711,16 +913,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -728,16 +930,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -745,16 +947,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -762,16 +964,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -779,16 +981,16 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -796,16 +998,16 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -813,16 +1015,16 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -830,16 +1032,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -847,16 +1049,16 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>112</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -864,16 +1066,16 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>113</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -881,13 +1083,16 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>114</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -895,13 +1100,16 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -909,16 +1117,16 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -926,16 +1134,16 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -943,16 +1151,16 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -960,16 +1168,16 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -977,149 +1185,839 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>120</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>121</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>133</v>
+      </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>135</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>133</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1</v>
+      </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>133</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>133</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
-        <v>64</v>
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>139</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>1</v>
+      </c>
       <c r="B23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" t="s">
-        <v>68</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>1</v>
+      </c>
       <c r="B24" t="s">
-        <v>88</v>
-      </c>
-      <c r="C24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" t="s">
-        <v>71</v>
+        <v>148</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>1</v>
+      </c>
       <c r="B25" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" t="s">
-        <v>72</v>
+        <v>148</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" t="s">
-        <v>76</v>
-      </c>
-      <c r="E26" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" t="s">
-        <v>79</v>
-      </c>
-      <c r="E27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" t="s">
-        <v>82</v>
-      </c>
-      <c r="E28" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
-        <v>84</v>
-      </c>
-      <c r="D29" t="s">
-        <v>82</v>
-      </c>
-      <c r="E29" t="s">
-        <v>85</v>
+        <v>146</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E450260-C86C-4E3F-B105-E3CAA65587BC}">
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>131</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>132</v>
+      </c>
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1974C2B-8E47-4949-A3F4-0096B87D2717}">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" activeCellId="1" sqref="A2:C2 A17:C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>